<commit_message>
Change: separate data and logic , Fix: updating excel sheet
</commit_message>
<xml_diff>
--- a/football_club_data.xlsx
+++ b/football_club_data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="75">
   <si>
     <t>ID</t>
   </si>
@@ -226,19 +226,19 @@
     <t>57.5</t>
   </si>
   <si>
-    <t>jj</t>
-  </si>
-  <si>
-    <t>hm</t>
-  </si>
-  <si>
-    <t>45.0</t>
-  </si>
-  <si>
     <t>r</t>
   </si>
   <si>
-    <t>3.0</t>
+    <t>m</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>nana</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
   <si>
     <t>Count</t>
@@ -1143,7 +1143,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1722079220336</v>
+        <v>1722093666927</v>
       </c>
       <c r="B21" t="s">
         <v>69</v>
@@ -1152,13 +1152,13 @@
         <v>70</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G21" t="s">
         <v>71</v>
@@ -1169,25 +1169,25 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1722090046821</v>
+        <v>1722093683411</v>
       </c>
       <c r="B22" t="s">
         <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H22" t="s">
         <v>22</v>
@@ -1201,7 +1201,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1306,110 +1306,6 @@
       </c>
       <c r="H4" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5">
-        <v>45</v>
-      </c>
-      <c r="E5">
-        <v>89</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1722079220336</v>
-      </c>
-      <c r="B6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>88</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7">
-        <v>88</v>
-      </c>
-      <c r="E7">
-        <v>87</v>
-      </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8">
-        <v>90</v>
-      </c>
-      <c r="E8">
-        <v>86</v>
-      </c>
-      <c r="F8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1420,7 +1316,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1451,106 +1347,28 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D2">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="E2">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="F2" t="s">
         <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3">
-        <v>45</v>
-      </c>
-      <c r="E3">
-        <v>89</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4">
-        <v>97</v>
-      </c>
-      <c r="E4">
-        <v>85</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5">
-        <v>85</v>
-      </c>
-      <c r="E5">
-        <v>79</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2129,25 +1947,25 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1722090046821</v>
+        <v>1722093666927</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H21" t="s">
         <v>22</v>
@@ -2155,22 +1973,22 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1722079220336</v>
+        <v>1722093683411</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G22" t="s">
         <v>71</v>
@@ -2281,25 +2099,25 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1722090046821</v>
+        <v>1722093666927</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H2" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Edit: console log statemenet
</commit_message>
<xml_diff>
--- a/football_club_data.xlsx
+++ b/football_club_data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="82">
   <si>
     <t>ID</t>
   </si>
@@ -251,6 +251,15 @@
   </si>
   <si>
     <t>barakat</t>
+  </si>
+  <si>
+    <t>Farah</t>
+  </si>
+  <si>
+    <t>Barakat</t>
+  </si>
+  <si>
+    <t>23.0</t>
   </si>
   <si>
     <t>Count</t>
@@ -630,7 +639,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1254,6 +1263,32 @@
         <v>71</v>
       </c>
       <c r="H24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1722160739577</v>
+      </c>
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25">
+        <v>12</v>
+      </c>
+      <c r="E25">
+        <v>34</v>
+      </c>
+      <c r="F25" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" t="s">
+        <v>80</v>
+      </c>
+      <c r="H25" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1265,7 +1300,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H10"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1369,6 +1404,162 @@
         <v>11</v>
       </c>
       <c r="H4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>45</v>
+      </c>
+      <c r="E5">
+        <v>89</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6">
+        <v>88</v>
+      </c>
+      <c r="E6">
+        <v>87</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7">
+        <v>90</v>
+      </c>
+      <c r="E7">
+        <v>86</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8">
+        <v>97</v>
+      </c>
+      <c r="E8">
+        <v>85</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>87</v>
+      </c>
+      <c r="E9">
+        <v>82</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10">
+        <v>85</v>
+      </c>
+      <c r="E10">
+        <v>79</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1380,7 +1571,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1411,28 +1602,54 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D2">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="E2">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="H2" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3">
+        <v>76</v>
+      </c>
+      <c r="E3">
+        <v>77</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1451,7 +1668,7 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1459,7 +1676,7 @@
         <v>22</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1486,7 +1703,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2011,25 +2228,25 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1722093666927</v>
+        <v>1722160739577</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="F21" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G21" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="H21" t="s">
         <v>22</v>
@@ -2037,13 +2254,13 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1722094926709</v>
+        <v>1722093683411</v>
       </c>
       <c r="B22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2063,13 +2280,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>1722093683411</v>
+        <v>1722095244591</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -2089,13 +2306,13 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>1722095244591</v>
+        <v>1722093666927</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -2110,6 +2327,32 @@
         <v>71</v>
       </c>
       <c r="H24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1722094926709</v>
+      </c>
+      <c r="B25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" t="s">
+        <v>71</v>
+      </c>
+      <c r="H25" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2215,13 +2458,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1722093666927</v>
+        <v>1722093683411</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D2">
         <v>1</v>

</xml_diff>

<commit_message>
ADD: all players using api call
</commit_message>
<xml_diff>
--- a/football_club_data.xlsx
+++ b/football_club_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="135">
   <si>
     <t>ID</t>
   </si>
@@ -117,6 +117,66 @@
     <t>Nazzal</t>
   </si>
   <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>91.0</t>
+  </si>
+  <si>
+    <t>Jacob</t>
+  </si>
+  <si>
+    <t>Stone</t>
+  </si>
+  <si>
+    <t>78.0</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Finley</t>
+  </si>
+  <si>
+    <t>Cross</t>
+  </si>
+  <si>
+    <t>89.0</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Chaffey</t>
+  </si>
+  <si>
+    <t>81.5</t>
+  </si>
+  <si>
+    <t>Joshua</t>
+  </si>
+  <si>
+    <t>Mills</t>
+  </si>
+  <si>
+    <t>Leander</t>
+  </si>
+  <si>
+    <t>Moore</t>
+  </si>
+  <si>
+    <t>Rashid</t>
+  </si>
+  <si>
+    <t>Bhatti</t>
+  </si>
+  <si>
+    <t>88.0</t>
+  </si>
+  <si>
     <t>Steven</t>
   </si>
   <si>
@@ -126,31 +186,208 @@
     <t>87.5</t>
   </si>
   <si>
-    <t>Rashid</t>
-  </si>
-  <si>
-    <t>Bhatti</t>
-  </si>
-  <si>
-    <t>88.0</t>
-  </si>
-  <si>
-    <t>Thomas</t>
-  </si>
-  <si>
-    <t>Taylor</t>
-  </si>
-  <si>
-    <t>91.0</t>
-  </si>
-  <si>
-    <t>Finley</t>
-  </si>
-  <si>
-    <t>Cross</t>
-  </si>
-  <si>
-    <t>89.0</t>
+    <t>Theo</t>
+  </si>
+  <si>
+    <t>Dolan</t>
+  </si>
+  <si>
+    <t>84.5</t>
+  </si>
+  <si>
+    <t>Alfie</t>
+  </si>
+  <si>
+    <t>Loy</t>
+  </si>
+  <si>
+    <t>82.0</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Adams</t>
+  </si>
+  <si>
+    <t>Isaac</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>76.5</t>
+  </si>
+  <si>
+    <t>Lucas</t>
+  </si>
+  <si>
+    <t>Saunders</t>
+  </si>
+  <si>
+    <t>68.5</t>
+  </si>
+  <si>
+    <t>Arlo</t>
+  </si>
+  <si>
+    <t>Gilchrist</t>
+  </si>
+  <si>
+    <t>57.5</t>
+  </si>
+  <si>
+    <t>najat</t>
+  </si>
+  <si>
+    <t>hasan</t>
+  </si>
+  <si>
+    <t>56.0</t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>Daly</t>
+  </si>
+  <si>
+    <t>55.0</t>
+  </si>
+  <si>
+    <t>zaynab</t>
+  </si>
+  <si>
+    <t>wehbe</t>
+  </si>
+  <si>
+    <t>45.0</t>
+  </si>
+  <si>
+    <t>Daher</t>
+  </si>
+  <si>
+    <t>34.0</t>
+  </si>
+  <si>
+    <t>rasha</t>
+  </si>
+  <si>
+    <t>malak</t>
+  </si>
+  <si>
+    <t>22.0</t>
+  </si>
+  <si>
+    <t>final</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>28.5</t>
+  </si>
+  <si>
+    <t>khalil</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>hhhh</t>
+  </si>
+  <si>
+    <t>lll</t>
+  </si>
+  <si>
+    <t>12.5</t>
+  </si>
+  <si>
+    <t>ttt</t>
+  </si>
+  <si>
+    <t>ee</t>
+  </si>
+  <si>
+    <t>12.0</t>
+  </si>
+  <si>
+    <t>Farah</t>
+  </si>
+  <si>
+    <t>Barakat</t>
+  </si>
+  <si>
+    <t>23.0</t>
+  </si>
+  <si>
+    <t>NASHLA TEZBAT</t>
+  </si>
+  <si>
+    <t>hope</t>
+  </si>
+  <si>
+    <t>17.5</t>
+  </si>
+  <si>
+    <t>yy</t>
+  </si>
+  <si>
+    <t>rt</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>hse</t>
+  </si>
+  <si>
+    <t>shah</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>tftr</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>tt</t>
+  </si>
+  <si>
+    <t>ooo</t>
+  </si>
+  <si>
+    <t>mmm</t>
+  </si>
+  <si>
+    <t>ppp</t>
+  </si>
+  <si>
+    <t>eee</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>nana</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>barakattt</t>
   </si>
   <si>
     <t>rana</t>
@@ -159,225 +396,6 @@
     <t>barakat</t>
   </si>
   <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>William</t>
-  </si>
-  <si>
-    <t>Adams</t>
-  </si>
-  <si>
-    <t>78.0</t>
-  </si>
-  <si>
-    <t>Jacob</t>
-  </si>
-  <si>
-    <t>Stone</t>
-  </si>
-  <si>
-    <t>Farah</t>
-  </si>
-  <si>
-    <t>Barakat</t>
-  </si>
-  <si>
-    <t>23.0</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>Chaffey</t>
-  </si>
-  <si>
-    <t>81.5</t>
-  </si>
-  <si>
-    <t>Joshua</t>
-  </si>
-  <si>
-    <t>Mills</t>
-  </si>
-  <si>
-    <t>Leander</t>
-  </si>
-  <si>
-    <t>Moore</t>
-  </si>
-  <si>
-    <t>Theo</t>
-  </si>
-  <si>
-    <t>Dolan</t>
-  </si>
-  <si>
-    <t>84.5</t>
-  </si>
-  <si>
-    <t>Alfie</t>
-  </si>
-  <si>
-    <t>Loy</t>
-  </si>
-  <si>
-    <t>82.0</t>
-  </si>
-  <si>
-    <t>Isaac</t>
-  </si>
-  <si>
-    <t>Johnson</t>
-  </si>
-  <si>
-    <t>76.5</t>
-  </si>
-  <si>
-    <t>Lucas</t>
-  </si>
-  <si>
-    <t>Saunders</t>
-  </si>
-  <si>
-    <t>68.5</t>
-  </si>
-  <si>
-    <t>Arlo</t>
-  </si>
-  <si>
-    <t>Gilchrist</t>
-  </si>
-  <si>
-    <t>57.5</t>
-  </si>
-  <si>
-    <t>najat</t>
-  </si>
-  <si>
-    <t>hasan</t>
-  </si>
-  <si>
-    <t>56.0</t>
-  </si>
-  <si>
-    <t>Alexander</t>
-  </si>
-  <si>
-    <t>Daly</t>
-  </si>
-  <si>
-    <t>55.0</t>
-  </si>
-  <si>
-    <t>zaynab</t>
-  </si>
-  <si>
-    <t>wehbe</t>
-  </si>
-  <si>
-    <t>45.0</t>
-  </si>
-  <si>
-    <t>Daher</t>
-  </si>
-  <si>
-    <t>34.0</t>
-  </si>
-  <si>
-    <t>rasha</t>
-  </si>
-  <si>
-    <t>malak</t>
-  </si>
-  <si>
-    <t>22.0</t>
-  </si>
-  <si>
-    <t>final</t>
-  </si>
-  <si>
-    <t>one</t>
-  </si>
-  <si>
-    <t>28.5</t>
-  </si>
-  <si>
-    <t>khalil</t>
-  </si>
-  <si>
-    <t>set</t>
-  </si>
-  <si>
-    <t>ttt</t>
-  </si>
-  <si>
-    <t>ee</t>
-  </si>
-  <si>
-    <t>12.0</t>
-  </si>
-  <si>
-    <t>NASHLA TEZBAT</t>
-  </si>
-  <si>
-    <t>hope</t>
-  </si>
-  <si>
-    <t>17.5</t>
-  </si>
-  <si>
-    <t>yy</t>
-  </si>
-  <si>
-    <t>rt</t>
-  </si>
-  <si>
-    <t>3.0</t>
-  </si>
-  <si>
-    <t>hse</t>
-  </si>
-  <si>
-    <t>shah</t>
-  </si>
-  <si>
-    <t>2.5</t>
-  </si>
-  <si>
-    <t>tftr</t>
-  </si>
-  <si>
-    <t>2.0</t>
-  </si>
-  <si>
-    <t>tt</t>
-  </si>
-  <si>
-    <t>ooo</t>
-  </si>
-  <si>
-    <t>mmm</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>nana</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>barakattt</t>
-  </si>
-  <si>
     <t>malouka</t>
   </si>
   <si>
@@ -388,9 +406,6 @@
   </si>
   <si>
     <t>gg</t>
-  </si>
-  <si>
-    <t>1.5</t>
   </si>
   <si>
     <t>finall</t>
@@ -785,7 +800,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H53"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1212,6 +1227,22 @@
       </c>
       <c r="G51">
         <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="G52">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="53" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <v>23</v>
+      </c>
+      <c r="G53">
+        <v>12.5</v>
       </c>
     </row>
   </sheetData>
@@ -1222,7 +1253,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1409,7 +1440,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>32</v>
@@ -1418,97 +1449,19 @@
         <v>33</v>
       </c>
       <c r="D8">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="E8">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="G8" t="s">
         <v>34</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9">
-        <v>90</v>
-      </c>
-      <c r="E9">
-        <v>86</v>
-      </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10">
-        <v>97</v>
-      </c>
-      <c r="E10">
-        <v>85</v>
-      </c>
-      <c r="F10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11">
-        <v>95</v>
-      </c>
-      <c r="E11">
-        <v>83</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1519,7 +1472,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1550,25 +1503,25 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1722095244591</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -1576,132 +1529,28 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="D3">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="E3">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4">
-        <v>45</v>
-      </c>
-      <c r="E4">
-        <v>89</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5">
-        <v>78</v>
-      </c>
-      <c r="E5">
-        <v>78</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6">
-        <v>77</v>
-      </c>
-      <c r="E6">
-        <v>79</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1722160739577</v>
-      </c>
-      <c r="B7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7">
-        <v>12</v>
-      </c>
-      <c r="E7">
-        <v>34</v>
-      </c>
-      <c r="F7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" t="s">
-        <v>54</v>
-      </c>
-      <c r="H7" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1720,7 +1569,7 @@
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1736,7 +1585,7 @@
         <v>22</v>
       </c>
       <c r="B3">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1755,7 +1604,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H53"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1815,10 +1664,10 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D3">
         <v>97</v>
@@ -1830,7 +1679,7 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H3" t="s">
         <v>12</v>
@@ -1841,10 +1690,10 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>95</v>
@@ -1856,7 +1705,7 @@
         <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H4" t="s">
         <v>22</v>
@@ -1867,10 +1716,10 @@
         <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>93</v>
@@ -1882,7 +1731,7 @@
         <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H5" t="s">
         <v>17</v>
@@ -1893,10 +1742,10 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D6">
         <v>92</v>
@@ -1908,7 +1757,7 @@
         <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H6" t="s">
         <v>17</v>
@@ -1919,10 +1768,10 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D7">
         <v>91</v>
@@ -1934,7 +1783,7 @@
         <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H7" t="s">
         <v>22</v>
@@ -1945,10 +1794,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D8">
         <v>90</v>
@@ -1960,7 +1809,7 @@
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="H8" t="s">
         <v>22</v>
@@ -1997,10 +1846,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="D10">
         <v>88</v>
@@ -2012,7 +1861,7 @@
         <v>28</v>
       </c>
       <c r="G10" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="H10" t="s">
         <v>22</v>
@@ -2023,10 +1872,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D11">
         <v>87</v>
@@ -2038,7 +1887,7 @@
         <v>15</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="H11" t="s">
         <v>17</v>
@@ -2049,10 +1898,10 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D12">
         <v>85</v>
@@ -2064,7 +1913,7 @@
         <v>28</v>
       </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="H12" t="s">
         <v>17</v>
@@ -2101,10 +1950,10 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D14">
         <v>78</v>
@@ -2116,7 +1965,7 @@
         <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="H14" t="s">
         <v>22</v>
@@ -2127,10 +1976,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D15">
         <v>77</v>
@@ -2142,7 +1991,7 @@
         <v>28</v>
       </c>
       <c r="G15" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="H15" t="s">
         <v>22</v>
@@ -2153,10 +2002,10 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D16">
         <v>76</v>
@@ -2168,7 +2017,7 @@
         <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H16" t="s">
         <v>12</v>
@@ -2179,10 +2028,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D17">
         <v>68</v>
@@ -2194,7 +2043,7 @@
         <v>28</v>
       </c>
       <c r="G17" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H17" t="s">
         <v>17</v>
@@ -2257,10 +2106,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D20">
         <v>50</v>
@@ -2272,7 +2121,7 @@
         <v>10</v>
       </c>
       <c r="G20" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H20" t="s">
         <v>17</v>
@@ -2309,10 +2158,10 @@
         <v>1722337556049</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D22">
         <v>45</v>
@@ -2324,7 +2173,7 @@
         <v>15</v>
       </c>
       <c r="G22" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H22" t="s">
         <v>22</v>
@@ -2335,10 +2184,10 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D23">
         <v>43</v>
@@ -2350,7 +2199,7 @@
         <v>10</v>
       </c>
       <c r="G23" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H23" t="s">
         <v>22</v>
@@ -2361,10 +2210,10 @@
         <v>1722341295181</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C24" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D24">
         <v>34</v>
@@ -2376,7 +2225,7 @@
         <v>15</v>
       </c>
       <c r="G24" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H24" t="s">
         <v>22</v>
@@ -2390,7 +2239,7 @@
         <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D25">
         <v>23</v>
@@ -2402,7 +2251,7 @@
         <v>20</v>
       </c>
       <c r="G25" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="H25" t="s">
         <v>12</v>
@@ -2413,10 +2262,10 @@
         <v>1722337948487</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D26">
         <v>23</v>
@@ -2428,7 +2277,7 @@
         <v>10</v>
       </c>
       <c r="G26" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="H26" t="s">
         <v>22</v>
@@ -2439,10 +2288,10 @@
         <v>1722338800317</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D27">
         <v>23</v>
@@ -2454,7 +2303,7 @@
         <v>20</v>
       </c>
       <c r="G27" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H27" t="s">
         <v>12</v>
@@ -2465,10 +2314,10 @@
         <v>1722339988206</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C28" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D28">
         <v>23</v>
@@ -2480,7 +2329,7 @@
         <v>20</v>
       </c>
       <c r="G28" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H28" t="s">
         <v>12</v>
@@ -2488,16 +2337,16 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>1722339327512</v>
+        <v>1722347177361</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C29" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D29">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E29">
         <v>2</v>
@@ -2506,7 +2355,7 @@
         <v>20</v>
       </c>
       <c r="G29" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="H29" t="s">
         <v>22</v>
@@ -2514,51 +2363,51 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>1722160739577</v>
+        <v>1722339327512</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="D30">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E30">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="F30" t="s">
         <v>20</v>
       </c>
       <c r="G30" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
       <c r="H30" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>1722338389197</v>
+        <v>1722160739577</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D31">
         <v>12</v>
       </c>
       <c r="E31">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="F31" t="s">
         <v>20</v>
       </c>
       <c r="G31" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H31" t="s">
         <v>12</v>
@@ -2566,42 +2415,42 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>1722338849343</v>
+        <v>1722338389197</v>
       </c>
       <c r="B32" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D32">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E32">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F32" t="s">
         <v>20</v>
       </c>
       <c r="G32" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H32" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>1722257968461</v>
+        <v>1722338849343</v>
       </c>
       <c r="B33" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C33" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E33">
         <v>3</v>
@@ -2610,7 +2459,7 @@
         <v>20</v>
       </c>
       <c r="G33" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H33" t="s">
         <v>17</v>
@@ -2618,39 +2467,39 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>1722261010188</v>
+        <v>1722257968461</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="C34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D34">
         <v>2</v>
       </c>
       <c r="E34">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F34" t="s">
         <v>20</v>
       </c>
       <c r="G34" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H34" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>1722338875827</v>
+        <v>1722261010188</v>
       </c>
       <c r="B35" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D35">
         <v>2</v>
@@ -2670,51 +2519,51 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>1722339287488</v>
+        <v>1722338875827</v>
       </c>
       <c r="B36" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="C36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D36">
         <v>2</v>
       </c>
       <c r="E36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F36" t="s">
         <v>20</v>
       </c>
       <c r="G36" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H36" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>1722093666927</v>
+        <v>1722339287488</v>
       </c>
       <c r="B37" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C37" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F37" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G37" t="s">
-        <v>46</v>
+        <v>108</v>
       </c>
       <c r="H37" t="s">
         <v>12</v>
@@ -2722,36 +2571,36 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>1722093683411</v>
+        <v>1722345736933</v>
       </c>
       <c r="B38" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" t="s">
+        <v>115</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G38" t="s">
         <v>116</v>
       </c>
-      <c r="C38" t="s">
-        <v>117</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38" t="s">
-        <v>10</v>
-      </c>
-      <c r="G38" t="s">
-        <v>46</v>
-      </c>
       <c r="H38" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>1722094926709</v>
+        <v>1722093666927</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C39" t="s">
         <v>118</v>
@@ -2766,7 +2615,7 @@
         <v>10</v>
       </c>
       <c r="G39" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="H39" t="s">
         <v>12</v>
@@ -2774,13 +2623,13 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>1722095244591</v>
+        <v>1722093683411</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="C40" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -2792,7 +2641,7 @@
         <v>10</v>
       </c>
       <c r="G40" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="H40" t="s">
         <v>12</v>
@@ -2800,13 +2649,13 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>1722254436153</v>
+        <v>1722094926709</v>
       </c>
       <c r="B41" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C41" t="s">
-        <v>79</v>
+        <v>122</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -2818,7 +2667,7 @@
         <v>10</v>
       </c>
       <c r="G41" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="H41" t="s">
         <v>12</v>
@@ -2826,13 +2675,13 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>1722257165295</v>
+        <v>1722095244591</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="C42" t="s">
-        <v>45</v>
+        <v>124</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -2844,7 +2693,7 @@
         <v>10</v>
       </c>
       <c r="G42" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="H42" t="s">
         <v>12</v>
@@ -2852,13 +2701,13 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>1722257311732</v>
+        <v>1722254436153</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C43" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="D43">
         <v>1</v>
@@ -2870,7 +2719,7 @@
         <v>10</v>
       </c>
       <c r="G43" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="H43" t="s">
         <v>12</v>
@@ -2878,13 +2727,13 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>1722260297301</v>
+        <v>1722257165295</v>
       </c>
       <c r="B44" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="C44" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -2896,7 +2745,7 @@
         <v>10</v>
       </c>
       <c r="G44" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="H44" t="s">
         <v>12</v>
@@ -2904,13 +2753,13 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>1722260461803</v>
+        <v>1722257311732</v>
       </c>
       <c r="B45" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="C45" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -2922,7 +2771,7 @@
         <v>10</v>
       </c>
       <c r="G45" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="H45" t="s">
         <v>12</v>
@@ -2930,13 +2779,13 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>1722335891851</v>
+        <v>1722260297301</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>125</v>
       </c>
       <c r="C46" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -2948,7 +2797,7 @@
         <v>10</v>
       </c>
       <c r="G46" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="H46" t="s">
         <v>12</v>
@@ -2956,13 +2805,13 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>1722335933734</v>
+        <v>1722260461803</v>
       </c>
       <c r="B47" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C47" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -2974,7 +2823,7 @@
         <v>10</v>
       </c>
       <c r="G47" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="H47" t="s">
         <v>12</v>
@@ -2982,65 +2831,65 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>1722337410001</v>
+        <v>1722335891851</v>
       </c>
       <c r="B48" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C48" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G48" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H48" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>1722338746639</v>
+        <v>1722335933734</v>
       </c>
       <c r="B49" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C49" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" t="s">
         <v>10</v>
       </c>
       <c r="G49" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H49" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>1722338819449</v>
+        <v>1722337410001</v>
       </c>
       <c r="B50" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="C50" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D50">
         <v>1</v>
@@ -3049,24 +2898,24 @@
         <v>2</v>
       </c>
       <c r="F50" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G50" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="H50" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>1722338961090</v>
+        <v>1722338746639</v>
       </c>
       <c r="B51" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C51" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -3075,12 +2924,64 @@
         <v>2</v>
       </c>
       <c r="F51" t="s">
+        <v>10</v>
+      </c>
+      <c r="G51" t="s">
+        <v>116</v>
+      </c>
+      <c r="H51" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1722338819449</v>
+      </c>
+      <c r="B52" t="s">
+        <v>131</v>
+      </c>
+      <c r="C52" t="s">
+        <v>132</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52" t="s">
+        <v>10</v>
+      </c>
+      <c r="G52" t="s">
+        <v>116</v>
+      </c>
+      <c r="H52" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1722338961090</v>
+      </c>
+      <c r="B53" t="s">
+        <v>133</v>
+      </c>
+      <c r="C53" t="s">
+        <v>134</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+      <c r="F53" t="s">
         <v>20</v>
       </c>
-      <c r="G51" t="s">
-        <v>123</v>
-      </c>
-      <c r="H51" t="s">
+      <c r="G53" t="s">
+        <v>116</v>
+      </c>
+      <c r="H53" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3189,10 +3090,10 @@
         <v>1722093666927</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -3204,7 +3105,7 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -3281,7 +3182,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -3310,32 +3211,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2">
-        <v>79</v>
-      </c>
-      <c r="E2">
-        <v>92</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>